<commit_message>
Scripts created from 208 to 214. Results - Pass
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -865,16 +865,16 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.8673469387755"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -957,7 +957,7 @@
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B21" s="10" t="n">
         <f aca="false">SUM(E3:E7)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1236,11 +1236,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,10 +1411,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,16 +1655,16 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.0969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,7 +1727,7 @@
         <v>103</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>104</v>
@@ -1738,7 +1738,7 @@
         <v>105</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>106</v>
@@ -1749,7 +1749,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>108</v>
@@ -1804,7 +1804,7 @@
         <v>117</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>118</v>
@@ -1815,7 +1815,7 @@
         <v>119</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>120</v>
@@ -1826,7 +1826,7 @@
         <v>121</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>122</v>
@@ -1837,7 +1837,7 @@
         <v>123</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>124</v>
@@ -1848,7 +1848,7 @@
         <v>125</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>126</v>
@@ -1977,10 +1977,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,10 +2106,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Scripts created-: IGP_TC_202 to IGP_TC_205. and IGP_TC_214 to IGP_TC_219
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -870,11 +870,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5969387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -957,7 +957,7 @@
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B21" s="10" t="n">
         <f aca="false">SUM(E3:E7)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1231,16 +1231,16 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,7 +1290,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>45</v>
@@ -1304,7 +1304,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>47</v>
@@ -1330,7 +1330,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>51</v>
@@ -1344,7 +1344,7 @@
         <v>52</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>53</v>
@@ -1358,7 +1358,7 @@
         <v>54</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>55</v>
@@ -1372,7 +1372,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>57</v>
@@ -1405,16 +1405,16 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,7 +1455,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>63</v>
@@ -1466,7 +1466,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>65</v>
@@ -1477,7 +1477,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>67</v>
@@ -1488,7 +1488,7 @@
         <v>68</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>69</v>
@@ -1499,18 +1499,18 @@
         <v>70</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>73</v>
@@ -1521,7 +1521,7 @@
         <v>74</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>75</v>
@@ -1532,29 +1532,29 @@
         <v>76</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
         <v>80</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>79</v>
@@ -1565,7 +1565,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>82</v>
@@ -1576,7 +1576,7 @@
         <v>83</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>84</v>
@@ -1587,7 +1587,7 @@
         <v>85</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>86</v>
@@ -1598,7 +1598,7 @@
         <v>87</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>88</v>
@@ -1609,7 +1609,7 @@
         <v>89</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>90</v>
@@ -1620,18 +1620,18 @@
         <v>91</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
         <v>93</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>94</v>
@@ -1655,16 +1655,16 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,18 +1859,18 @@
         <v>127</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
         <v>129</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>130</v>
@@ -1881,7 +1881,7 @@
         <v>131</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>132</v>
@@ -1892,7 +1892,7 @@
         <v>133</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>134</v>
@@ -1903,7 +1903,7 @@
         <v>135</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>136</v>
@@ -1914,7 +1914,7 @@
         <v>137</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C23" s="23" t="s">
         <v>138</v>
@@ -1925,7 +1925,7 @@
         <v>139</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C24" s="23" t="s">
         <v>140</v>
@@ -1942,12 +1942,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
         <v>143</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>144</v>
@@ -1977,10 +1977,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,10 +2106,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Scripts created -: IGP_TC_082.java, IGP_TC_083.java, IGP_TC_084.java
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" state="visible" r:id="rId2"/>
@@ -76,13 +76,13 @@
     <t xml:space="preserve">Payment</t>
   </si>
   <si>
+    <t xml:space="preserve">Suite3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order Summary Page</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order Detail Page</t>
   </si>
   <si>
     <t xml:space="preserve">Suite4</t>
@@ -864,17 +864,17 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3265306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -947,25 +947,25 @@
         <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>9</v>
@@ -975,7 +975,7 @@
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B21" s="10" t="n">
         <f aca="false">SUM(E3:E7)</f>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1156,7 +1156,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1167,7 +1167,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1178,7 +1178,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1236,11 +1236,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,7 +1262,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>40</v>
@@ -1276,7 +1276,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>43</v>
@@ -1290,7 +1290,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>45</v>
@@ -1304,7 +1304,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>47</v>
@@ -1330,7 +1330,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>51</v>
@@ -1344,7 +1344,7 @@
         <v>52</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>53</v>
@@ -1358,7 +1358,7 @@
         <v>54</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>55</v>
@@ -1372,7 +1372,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>57</v>
@@ -1411,10 +1411,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.6224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,7 +1433,7 @@
         <v>58</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>59</v>
@@ -1444,7 +1444,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>61</v>
@@ -1455,7 +1455,7 @@
         <v>62</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>63</v>
@@ -1466,7 +1466,7 @@
         <v>64</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>65</v>
@@ -1477,7 +1477,7 @@
         <v>66</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>67</v>
@@ -1488,7 +1488,7 @@
         <v>68</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>69</v>
@@ -1499,7 +1499,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>71</v>
@@ -1510,7 +1510,7 @@
         <v>72</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>73</v>
@@ -1521,7 +1521,7 @@
         <v>74</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>75</v>
@@ -1532,7 +1532,7 @@
         <v>76</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>77</v>
@@ -1543,7 +1543,7 @@
         <v>78</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>79</v>
@@ -1554,7 +1554,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>79</v>
@@ -1565,7 +1565,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>82</v>
@@ -1576,7 +1576,7 @@
         <v>83</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>84</v>
@@ -1587,7 +1587,7 @@
         <v>85</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>86</v>
@@ -1598,7 +1598,7 @@
         <v>87</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>88</v>
@@ -1609,7 +1609,7 @@
         <v>89</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>90</v>
@@ -1620,7 +1620,7 @@
         <v>91</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>92</v>
@@ -1631,7 +1631,7 @@
         <v>93</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>94</v>
@@ -1655,16 +1655,16 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.9387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1683,7 +1683,7 @@
         <v>95</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>96</v>
@@ -1694,7 +1694,7 @@
         <v>97</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>98</v>
@@ -1705,7 +1705,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>100</v>
@@ -1716,7 +1716,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>102</v>
@@ -1727,7 +1727,7 @@
         <v>103</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>104</v>
@@ -1738,7 +1738,7 @@
         <v>105</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>106</v>
@@ -1749,7 +1749,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>108</v>
@@ -1804,7 +1804,7 @@
         <v>117</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>118</v>
@@ -1815,7 +1815,7 @@
         <v>119</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>120</v>
@@ -1826,7 +1826,7 @@
         <v>121</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>122</v>
@@ -1837,7 +1837,7 @@
         <v>123</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>124</v>
@@ -1848,7 +1848,7 @@
         <v>125</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>126</v>
@@ -1859,7 +1859,7 @@
         <v>127</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>128</v>
@@ -1870,7 +1870,7 @@
         <v>129</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>130</v>
@@ -1881,7 +1881,7 @@
         <v>131</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>132</v>
@@ -1892,7 +1892,7 @@
         <v>133</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>134</v>
@@ -1903,7 +1903,7 @@
         <v>135</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>136</v>
@@ -1914,7 +1914,7 @@
         <v>137</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C23" s="23" t="s">
         <v>138</v>
@@ -1925,7 +1925,7 @@
         <v>139</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C24" s="23" t="s">
         <v>140</v>
@@ -1947,7 +1947,7 @@
         <v>143</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>144</v>
@@ -1972,15 +1972,15 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.2908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1999,29 +1999,29 @@
         <v>145</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>147</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
         <v>149</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>150</v>
@@ -2106,10 +2106,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Script created for PDP
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Suite3" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Suite4" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Suite5" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Suite6" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Suite1" vbProcedure="false">Suite1!$A$1:$C$11</definedName>
@@ -25,14 +26,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="176">
   <si>
     <t xml:space="preserve">Project ID/Name</t>
   </si>
@@ -58,18 +59,21 @@
     <t xml:space="preserve">Cart page</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checkout Page</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">Chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checkout Page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Suite2</t>
   </si>
   <si>
@@ -88,15 +92,18 @@
     <t xml:space="preserve">URL Tests</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">REST</t>
   </si>
   <si>
     <t xml:space="preserve">Suite5</t>
   </si>
   <si>
+    <t xml:space="preserve">Product Description Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite6</t>
+  </si>
+  <si>
     <t xml:space="preserve">SETTINGS</t>
   </si>
   <si>
@@ -523,7 +530,37 @@
     <t xml:space="preserve">IGP_TC_URL</t>
   </si>
   <si>
-    <t xml:space="preserve">IGP URL Tests</t>
+    <t xml:space="preserve">IGP url test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin code validation:Ensure that the pin code box is accepting more than 6 digits, alphabets &amp; special symbols or not.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Area Pin code validation: Ensure that error message is coming for places where delivery is not supported.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International shipping: 'Enter Country name' field: Ensure that Enter Country name field should not accept numbers &amp; special symbols.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image of the gift:Ensure that the Image box should be in the left of the product description page and it has to display multiple thumbnails in different angles of the gift below it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoom in feature on the image:Ensure that when the user  mouse hover on image, it Should zoom in.</t>
   </si>
 </sst>
 </file>
@@ -561,7 +598,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -569,14 +606,14 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -598,7 +635,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -670,7 +707,7 @@
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -693,28 +730,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -722,31 +759,31 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -758,7 +795,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -799,6 +836,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -882,20 +927,20 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.0204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.6275510204082"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3061224489796"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -906,7 +951,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -923,7 +968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -938,48 +983,48 @@
       </c>
       <c r="E3" s="6" t="n">
         <f aca="false">IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6" t="n">
         <f aca="false">IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
@@ -988,19 +1033,19 @@
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="7" t="s">
         <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>19</v>
@@ -1010,15 +1055,26 @@
       </c>
       <c r="E7" s="6" t="n">
         <f aca="false">IF(B7="Y",COUNTIF(Suite5!B2:B51,"Y"),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <f aca="false">IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
@@ -1069,40 +1125,40 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>9</v>
@@ -1111,91 +1167,91 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B21" s="10" t="n">
-        <f aca="false">SUM(E3:E7)</f>
-        <v>1</v>
+        <f aca="false">SUM(E3:E15)</f>
+        <v>22</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1208,21 +1264,21 @@
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1231,7 +1287,7 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1248,165 +1304,165 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
       <c r="B11" s="19"/>
       <c r="C11" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1422,244 +1478,244 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1676,380 +1732,380 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2091836734694"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2071,141 +2127,132 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>41</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2230,40 +2277,40 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2275,4 +2322,207 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.04591836734694"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" s="27" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="18"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="18"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="18"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Scripts created for PDP
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="182">
   <si>
     <t xml:space="preserve">Project ID/Name</t>
   </si>
@@ -59,48 +59,48 @@
     <t xml:space="preserve">Cart page</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checkout Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order Summary Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL Tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suite5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Description Page</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checkout Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order Summary Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URL Tests</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suite5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Description Page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Suite6</t>
   </si>
   <si>
@@ -561,6 +561,24 @@
   </si>
   <si>
     <t xml:space="preserve">Zoom in feature on the image:Ensure that when the user  mouse hover on image, it Should zoom in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product name and Price-:Ensure that the selected product name and price   should be same with what we are selected in listing page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size option-: Ensure that the Size option displayed when size variants exist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need Help?-:Ensure that user able to send query by clicking on 'Need Help' from the "Product Description" page.</t>
   </si>
 </sst>
 </file>
@@ -926,17 +944,17 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.0204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.0357142857143"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -983,7 +1001,7 @@
       </c>
       <c r="E3" s="6" t="n">
         <f aca="false">IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,13 +1009,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="6" t="n">
         <f aca="false">IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
@@ -1006,16 +1024,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
@@ -1024,7 +1042,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
@@ -1033,25 +1051,25 @@
         <v>9</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="6" t="n">
         <f aca="false">IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="E7" s="6" t="n">
         <f aca="false">IF(B7="Y",COUNTIF(Suite5!B2:B51,"Y"),0)</f>
@@ -1060,10 +1078,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>9</v>
@@ -1073,7 +1091,7 @@
       </c>
       <c r="E8" s="6" t="n">
         <f aca="false">IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,7 +1190,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1184,7 +1202,7 @@
       </c>
       <c r="B21" s="10" t="n">
         <f aca="false">SUM(E3:E15)</f>
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1229,7 +1247,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1240,7 +1258,7 @@
         <v>35</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1251,7 +1269,7 @@
         <v>36</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1309,11 +1327,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7397959183673"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,7 +1353,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>42</v>
@@ -1349,7 +1367,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>45</v>
@@ -1363,7 +1381,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>47</v>
@@ -1377,7 +1395,7 @@
         <v>48</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>49</v>
@@ -1391,7 +1409,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>51</v>
@@ -1403,7 +1421,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>53</v>
@@ -1417,7 +1435,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>55</v>
@@ -1431,7 +1449,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>57</v>
@@ -1445,7 +1463,7 @@
         <v>58</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>59</v>
@@ -1484,10 +1502,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,7 +1527,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>61</v>
@@ -1520,7 +1538,7 @@
         <v>62</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>63</v>
@@ -1531,7 +1549,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>65</v>
@@ -1542,7 +1560,7 @@
         <v>66</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>67</v>
@@ -1553,7 +1571,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>69</v>
@@ -1564,7 +1582,7 @@
         <v>70</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>71</v>
@@ -1575,7 +1593,7 @@
         <v>72</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>73</v>
@@ -1586,7 +1604,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>75</v>
@@ -1597,7 +1615,7 @@
         <v>76</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>77</v>
@@ -1608,7 +1626,7 @@
         <v>78</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>79</v>
@@ -1619,7 +1637,7 @@
         <v>80</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>81</v>
@@ -1630,7 +1648,7 @@
         <v>82</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>81</v>
@@ -1641,7 +1659,7 @@
         <v>83</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>84</v>
@@ -1652,7 +1670,7 @@
         <v>85</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>86</v>
@@ -1663,7 +1681,7 @@
         <v>87</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>88</v>
@@ -1674,7 +1692,7 @@
         <v>89</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>90</v>
@@ -1685,7 +1703,7 @@
         <v>91</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>92</v>
@@ -1696,7 +1714,7 @@
         <v>93</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>94</v>
@@ -1707,7 +1725,7 @@
         <v>95</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>96</v>
@@ -1737,11 +1755,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,7 +1781,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>98</v>
@@ -1777,7 +1795,7 @@
         <v>99</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>100</v>
@@ -1791,7 +1809,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>102</v>
@@ -1805,7 +1823,7 @@
         <v>103</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>104</v>
@@ -1819,7 +1837,7 @@
         <v>105</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>106</v>
@@ -1833,7 +1851,7 @@
         <v>107</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>108</v>
@@ -1847,7 +1865,7 @@
         <v>109</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>110</v>
@@ -1861,7 +1879,7 @@
         <v>111</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>112</v>
@@ -1875,7 +1893,7 @@
         <v>113</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>114</v>
@@ -1889,7 +1907,7 @@
         <v>115</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>116</v>
@@ -1903,7 +1921,7 @@
         <v>117</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>118</v>
@@ -1917,7 +1935,7 @@
         <v>119</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>120</v>
@@ -1931,7 +1949,7 @@
         <v>121</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>122</v>
@@ -1945,7 +1963,7 @@
         <v>123</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>124</v>
@@ -1959,7 +1977,7 @@
         <v>125</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>126</v>
@@ -1973,7 +1991,7 @@
         <v>127</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>128</v>
@@ -1987,7 +2005,7 @@
         <v>129</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>130</v>
@@ -2001,7 +2019,7 @@
         <v>131</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>132</v>
@@ -2015,7 +2033,7 @@
         <v>133</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>134</v>
@@ -2029,7 +2047,7 @@
         <v>135</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>136</v>
@@ -2043,7 +2061,7 @@
         <v>137</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C22" s="23" t="s">
         <v>138</v>
@@ -2057,7 +2075,7 @@
         <v>139</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C23" s="23" t="s">
         <v>140</v>
@@ -2071,7 +2089,7 @@
         <v>141</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C24" s="23" t="s">
         <v>142</v>
@@ -2085,7 +2103,7 @@
         <v>143</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>144</v>
@@ -2099,7 +2117,7 @@
         <v>146</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>147</v>
@@ -2132,10 +2150,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2157,7 +2175,7 @@
         <v>148</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>149</v>
@@ -2171,7 +2189,7 @@
         <v>150</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>151</v>
@@ -2185,7 +2203,7 @@
         <v>152</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>153</v>
@@ -2199,7 +2217,7 @@
         <v>154</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>155</v>
@@ -2213,7 +2231,7 @@
         <v>156</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>157</v>
@@ -2227,7 +2245,7 @@
         <v>158</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>159</v>
@@ -2238,7 +2256,7 @@
         <v>160</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>161</v>
@@ -2249,7 +2267,7 @@
         <v>162</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>163</v>
@@ -2279,10 +2297,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,7 +2322,7 @@
         <v>164</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>165</v>
@@ -2331,15 +2349,15 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,7 +2379,7 @@
         <v>166</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>167</v>
@@ -2375,7 +2393,7 @@
         <v>168</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>169</v>
@@ -2389,7 +2407,7 @@
         <v>170</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>171</v>
@@ -2403,7 +2421,7 @@
         <v>172</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>173</v>
@@ -2412,12 +2430,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
         <v>174</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>175</v>
@@ -2426,23 +2444,47 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="18"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="18"/>
+    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>

</xml_diff>

<commit_message>
Scirpts created for PDP
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="191">
   <si>
     <t xml:space="preserve">Project ID/Name</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t xml:space="preserve">Merge cart items: Ensure that items in the cart merged upon user logged in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INVALID TC</t>
   </si>
   <si>
     <t xml:space="preserve">IGP_TC_095</t>
@@ -617,6 +620,12 @@
       </rPr>
       <t xml:space="preserve"> Ensure that user should not navigate to the next page with out completing all the steps in 'personalize now'.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP_TC_114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy without 'Personalizing' the gift-: Ensure with out personalizing the product when user click on Buy now , it should not navigate.</t>
   </si>
 </sst>
 </file>
@@ -991,16 +1000,16 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0867346938776"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -1047,7 +1056,7 @@
       </c>
       <c r="E3" s="6" t="n">
         <f aca="false">IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,7 +1092,7 @@
       </c>
       <c r="E5" s="6" t="n">
         <f aca="false">IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,7 +1146,7 @@
       </c>
       <c r="E8" s="6" t="n">
         <f aca="false">IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,7 +1257,7 @@
       </c>
       <c r="B21" s="10" t="n">
         <f aca="false">SUM(E3:E15)</f>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
@@ -1367,17 +1376,16 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.7142857142857"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="14" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,22 +1463,24 @@
         <v>50</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="0"/>
+      <c r="D6" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>43</v>
@@ -1478,13 +1488,13 @@
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>43</v>
@@ -1492,13 +1502,13 @@
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>43</v>
@@ -1506,13 +1516,13 @@
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>43</v>
@@ -1548,10 +1558,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.1989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,211 +1579,211 @@
     </row>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1795,17 +1804,16 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="13" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.1887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,353 +1830,353 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>101</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>105</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>107</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>113</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>123</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>125</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>127</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>131</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B20" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>135</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>137</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>141</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>143</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="0" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D25" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="D26" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2191,15 +2199,13 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.3265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,13 +2224,13 @@
     </row>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>43</v>
@@ -2232,13 +2238,13 @@
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>43</v>
@@ -2246,13 +2252,13 @@
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D4" s="25" t="s">
         <v>43</v>
@@ -2260,13 +2266,13 @@
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>43</v>
@@ -2274,13 +2280,13 @@
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>43</v>
@@ -2288,35 +2294,44 @@
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>161</v>
+        <v>162</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2343,10 +2358,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,13 +2380,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>43</v>
@@ -2395,15 +2410,15 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.4132653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2422,13 +2437,13 @@
     </row>
     <row r="2" s="27" customFormat="true" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D2" s="26" t="s">
         <v>43</v>
@@ -2436,13 +2451,13 @@
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>43</v>
@@ -2450,13 +2465,13 @@
     </row>
     <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>43</v>
@@ -2464,13 +2479,13 @@
     </row>
     <row r="5" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>43</v>
@@ -2478,13 +2493,13 @@
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>43</v>
@@ -2492,13 +2507,13 @@
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>43</v>
@@ -2506,13 +2521,13 @@
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>43</v>
@@ -2520,13 +2535,13 @@
     </row>
     <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>43</v>
@@ -2534,13 +2549,13 @@
     </row>
     <row r="10" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>43</v>
@@ -2548,13 +2563,13 @@
     </row>
     <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>43</v>
@@ -2562,23 +2577,31 @@
     </row>
     <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="18"/>
+    <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="18"/>

</xml_diff>

<commit_message>
Product Listing as well as Product Strip test strips are updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Suite4" sheetId="5" r:id="rId5"/>
     <sheet name="Suite5" sheetId="6" r:id="rId6"/>
     <sheet name="Suite6" sheetId="7" r:id="rId7"/>
+    <sheet name="Suite7" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="Suite1">Suite1!$A$1:$C$11</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -93,10 +94,16 @@
     <t>Product Description Page</t>
   </si>
   <si>
+    <t>Suite6</t>
+  </si>
+  <si>
+    <t>Product Listing Page</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Suite6</t>
+    <t>Suite7</t>
   </si>
   <si>
     <t>SETTINGS</t>
@@ -632,16 +639,46 @@
   <si>
     <t>Shipping charges for international delivery: Ensure that there should be Shipping charges for international delivery.</t>
   </si>
+  <si>
+    <t>IGP_TC_117</t>
+  </si>
+  <si>
+    <t>Free shipping to US and not shippable to other countries: Ensure that the items which are shippable to US are not shippable to other countries.</t>
+  </si>
+  <si>
+    <t>IGP_TC_118</t>
+  </si>
+  <si>
+    <t>Free shipping to all countries but not shippable to US: Ensure that the items which are shippable to other countries are not shippable to US.</t>
+  </si>
+  <si>
+    <t>IGP_TC_232</t>
+  </si>
+  <si>
+    <t>Navigate to Product Listing page:User is able to see all the details on Product Listing Page for Birthday Card.</t>
+  </si>
+  <si>
+    <t>IGP_TC_233</t>
+  </si>
+  <si>
+    <t>Navigate to Product Listing page:User is able to see all the details on Product Listing Page for Women.</t>
+  </si>
+  <si>
+    <t>IGP_TC_234</t>
+  </si>
+  <si>
+    <t>Navigate to Product Listing page:User is able to see all the details on Product Listing Page for Anniversary Gifts.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -714,10 +751,49 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -730,22 +806,42 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -760,7 +856,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -768,36 +864,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -806,21 +873,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -836,22 +888,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -885,7 +922,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -897,19 +994,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,25 +1024,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -951,13 +1042,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -969,7 +1072,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -981,49 +1090,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1035,37 +1102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1109,17 +1146,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1149,6 +1180,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1159,6 +1205,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1180,15 +1235,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1197,21 +1243,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1219,134 +1256,134 @@
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1362,17 +1399,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1819,363 +1862,373 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="31.8571428571429" style="18"/>
-    <col min="2" max="2" width="17.2761904761905" style="18"/>
-    <col min="3" max="3" width="8.37142857142857" style="18"/>
-    <col min="4" max="4" width="6.07619047619048" style="18"/>
-    <col min="5" max="5" width="18.0857142857143" style="18"/>
-    <col min="6" max="1025" width="6.07619047619048" style="18"/>
+    <col min="1" max="1" width="31.8571428571429" style="20"/>
+    <col min="2" max="2" width="17.2761904761905" style="20"/>
+    <col min="3" max="3" width="8.37142857142857" style="20"/>
+    <col min="4" max="4" width="6.07619047619048" style="20"/>
+    <col min="5" max="5" width="18.0857142857143" style="20"/>
+    <col min="6" max="1025" width="6.07619047619048" style="20"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" ht="15.75" spans="1:5">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:5">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="25">
         <f>IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:5">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="25">
         <f>IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:5">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="25">
         <f>IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:5">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="25">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:5">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="25">
         <f>IF(B7="Y",COUNTIF(Suite5!B2:B51,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:5">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="E8" s="25">
+        <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="23">
-        <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="D9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="19">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" ht="15.75" spans="1:5">
-      <c r="A16" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="A16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" ht="15.75" spans="1:5">
-      <c r="A17" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" ht="15.75" spans="1:5">
-      <c r="A18" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="A18" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" ht="15.75" spans="1:5">
-      <c r="A19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="25" t="s">
+      <c r="A19" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" ht="15.75" spans="1:5">
-      <c r="A20" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="25" t="s">
+      <c r="A20" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" ht="15.75" spans="1:5">
-      <c r="A21" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="26">
+      <c r="A21" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="28">
         <f>SUM(E3:E15)</f>
-        <v>2</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="17"/>
+        <v>3</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" ht="15.75" spans="1:5">
-      <c r="A22" s="24"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="17"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="17"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="17"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="19"/>
     </row>
     <row r="24" ht="15.75" spans="1:5">
-      <c r="A24" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
+      <c r="A24" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" ht="15.75" spans="1:5">
-      <c r="A25" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="A25" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" ht="15.75" spans="1:5">
-      <c r="A26" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="A26" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" ht="15.75" spans="1:5">
-      <c r="A27" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="A27" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" ht="15.75" spans="1:5">
-      <c r="A28" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
+      <c r="A28" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" ht="15.75" spans="1:5">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" ht="15.75" spans="1:5">
-      <c r="A31" s="24"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" ht="15.75" spans="1:5">
-      <c r="A32" s="24"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
@@ -2196,156 +2249,156 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="12.4190476190476"/>
-    <col min="2" max="2" width="6.07619047619048" style="10"/>
+    <col min="2" max="2" width="6.07619047619048" style="12"/>
     <col min="3" max="3" width="41.7142857142857"/>
-    <col min="4" max="4" width="6.07619047619048" style="14"/>
+    <col min="4" max="4" width="6.07619047619048" style="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" ht="45" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>45</v>
+      <c r="A3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="45" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>47</v>
+      <c r="A4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>49</v>
+      <c r="A5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" ht="30" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="A6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>51</v>
+      <c r="C6" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" ht="30" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>54</v>
+      <c r="A7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" ht="45" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>56</v>
+      <c r="A8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="45" spans="1:4">
-      <c r="A9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>58</v>
+      <c r="A9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" ht="45" spans="1:8">
-      <c r="A10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="16"/>
+      <c r="A10" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
@@ -2366,231 +2419,231 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9.99047619047619"/>
-    <col min="2" max="2" width="6.07619047619048" style="10"/>
+    <col min="2" max="2" width="6.07619047619048" style="12"/>
     <col min="3" max="3" width="43.2"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>62</v>
+      <c r="A2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>64</v>
+      <c r="A3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" ht="60" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>66</v>
+      <c r="A4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" ht="60" spans="1:3">
-      <c r="A5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>68</v>
+      <c r="A5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" ht="30" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>70</v>
+      <c r="A6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" ht="45" spans="1:3">
-      <c r="A7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>72</v>
+      <c r="A7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" ht="45" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>74</v>
+      <c r="A8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" ht="45" spans="1:3">
-      <c r="A9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>76</v>
+      <c r="A9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="10" ht="60" spans="1:3">
-      <c r="A10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>78</v>
+      <c r="A10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" ht="30" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>80</v>
+      <c r="A11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" ht="45" spans="1:3">
-      <c r="A12" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>82</v>
+      <c r="A12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" ht="45" spans="1:3">
-      <c r="A13" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>82</v>
+      <c r="A13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="14" ht="60" spans="1:3">
-      <c r="A14" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>85</v>
+      <c r="A14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" ht="60" spans="1:3">
-      <c r="A15" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>87</v>
+      <c r="A15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="16" ht="60" spans="1:3">
-      <c r="A16" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>89</v>
+      <c r="A16" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" ht="60" spans="1:3">
-      <c r="A17" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>91</v>
+      <c r="A17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18" ht="60" spans="1:3">
-      <c r="A18" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>93</v>
+      <c r="A18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="19" ht="60" spans="1:3">
-      <c r="A19" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>95</v>
+      <c r="A19" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20" ht="45" spans="1:3">
-      <c r="A20" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>97</v>
+      <c r="A20" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2612,373 +2665,373 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="10.6666666666667"/>
-    <col min="2" max="2" width="6.07619047619048" style="10"/>
+    <col min="2" max="2" width="6.07619047619048" style="12"/>
     <col min="3" max="3" width="51.9714285714286"/>
     <col min="4" max="4" width="9.99047619047619"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>43</v>
+      <c r="A2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" ht="30" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>43</v>
+      <c r="A3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="30" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>43</v>
+      <c r="A4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" ht="45" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>43</v>
+      <c r="A5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>43</v>
+      <c r="A6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" ht="45" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>43</v>
+      <c r="A7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" ht="45" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>43</v>
+      <c r="A8" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="30" spans="1:4">
-      <c r="A9" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>43</v>
+      <c r="A9" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" ht="45" spans="1:4">
-      <c r="A10" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>43</v>
+      <c r="A10" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" ht="45" spans="1:4">
-      <c r="A11" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>43</v>
+      <c r="A11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" ht="60" spans="1:4">
-      <c r="A12" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
+      <c r="A12" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" ht="30" spans="1:4">
-      <c r="A13" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
+      <c r="A13" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" ht="30" spans="1:4">
-      <c r="A14" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>43</v>
+      <c r="A14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" ht="30" spans="1:4">
-      <c r="A15" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>43</v>
+      <c r="A15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" ht="30" spans="1:4">
-      <c r="A16" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>43</v>
+      <c r="A16" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" ht="30" spans="1:4">
-      <c r="A17" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>43</v>
+      <c r="A17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" ht="30" spans="1:4">
-      <c r="A18" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>43</v>
+      <c r="A18" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" ht="45" spans="1:4">
-      <c r="A19" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>43</v>
+      <c r="A19" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" ht="30" spans="1:4">
-      <c r="A20" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>43</v>
+      <c r="A20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" ht="30" spans="1:4">
-      <c r="A21" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>43</v>
+      <c r="A21" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" ht="30" spans="1:4">
-      <c r="A22" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>43</v>
+      <c r="A22" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" ht="30" spans="1:4">
-      <c r="A23" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>43</v>
+      <c r="A23" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" ht="30" spans="1:4">
-      <c r="A24" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>43</v>
+      <c r="A24" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" ht="30" spans="1:4">
-      <c r="A25" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="11" t="s">
+      <c r="A25" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>146</v>
+      <c r="C25" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="26" ht="45" spans="1:4">
-      <c r="A26" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>43</v>
+      <c r="A26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3008,128 +3061,128 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>43</v>
+      <c r="A2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>43</v>
+      <c r="A3" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="30" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>43</v>
+      <c r="A4" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>43</v>
+      <c r="A5" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" ht="30" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>43</v>
+      <c r="A6" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" ht="30" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>160</v>
+      <c r="A7" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" ht="30" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>162</v>
+      <c r="A8" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>164</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="30" spans="1:4">
-      <c r="A9" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>164</v>
+      <c r="A9" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3161,30 +3214,30 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3202,8 +3255,8 @@
   <sheetPr/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3215,253 +3268,376 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="45" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" s="9" customFormat="1" ht="45" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>43</v>
+      <c r="C2" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>43</v>
+      <c r="C3" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="45" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>43</v>
+      <c r="C4" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" ht="60" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>43</v>
+      <c r="C5" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>43</v>
+      <c r="C6" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" ht="45" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>43</v>
+      <c r="C7" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" ht="30" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>43</v>
+      <c r="C8" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" ht="45" spans="1:4">
-      <c r="A9" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>43</v>
+      <c r="C9" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" ht="60" spans="1:4">
-      <c r="A10" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>43</v>
+      <c r="C10" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" ht="45" spans="1:4">
-      <c r="A11" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>43</v>
+      <c r="C11" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" ht="45" spans="1:4">
-      <c r="A12" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>43</v>
+      <c r="C12" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" ht="45" spans="1:4">
-      <c r="A13" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
+      <c r="C13" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" ht="30" spans="1:4">
-      <c r="A14" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>43</v>
+      <c r="A14" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" ht="45" spans="1:4">
-      <c r="A15" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
+      <c r="A15" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" ht="60" spans="1:4">
+      <c r="A16" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" ht="45" spans="1:4">
+      <c r="A17" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" ht="45" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" ht="45" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" ht="45" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="10.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="21.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="95" customHeight="1" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="90" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="93" customHeight="1" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Case 240 created
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -96,13 +96,13 @@
     <t>Product Description Page</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>Suite6</t>
   </si>
   <si>
     <t>Product Listing Page</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>Suite7</t>
@@ -725,10 +725,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -796,13 +796,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -810,6 +805,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -823,18 +826,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -854,16 +907,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -878,17 +923,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -899,46 +937,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -972,19 +972,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -996,25 +990,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,49 +1032,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1092,7 +1062,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1104,7 +1122,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1116,43 +1134,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,11 +1196,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1220,26 +1226,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1277,8 +1268,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1293,164 +1284,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1921,391 +1915,393 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="31.8571428571429" style="23"/>
-    <col min="2" max="2" width="17.2761904761905" style="23"/>
-    <col min="3" max="3" width="8.37142857142857" style="23"/>
-    <col min="4" max="4" width="6.07619047619048" style="23"/>
-    <col min="5" max="5" width="18.0857142857143" style="23"/>
-    <col min="6" max="1025" width="6.07619047619048" style="23"/>
+    <col min="1" max="1" width="31.8571428571429" style="21"/>
+    <col min="2" max="2" width="17.2761904761905" style="21"/>
+    <col min="3" max="3" width="8.37142857142857" style="21"/>
+    <col min="4" max="4" width="6.07619047619048" style="21"/>
+    <col min="5" max="5" width="18.0857142857143" style="21"/>
+    <col min="6" max="1025" width="6.07619047619048" style="21"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" ht="15.75" spans="1:5">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:5">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <f>IF(B3="Y",COUNTIF(Suite1!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:5">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="26">
         <f>IF(B4="Y",COUNTIF(Suite2!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:5">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="26">
         <f>IF(B5="Y",COUNTIF(Suite3!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:5">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E6" s="26">
         <f>IF(B6="Y",COUNTIF(Suite4!B2:B50,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="15.75" spans="1:5">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="26">
         <f>IF(B7="Y",COUNTIF(Suite5!B2:B51,"Y"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" ht="15.75" spans="1:5">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="26">
+        <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" ht="15.75" spans="1:5">
+      <c r="A16" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" ht="15.75" spans="1:5">
+      <c r="A17" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" ht="15.75" spans="1:5">
+      <c r="A18" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" ht="15.75" spans="1:5">
+      <c r="A19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" ht="15.75" spans="1:5">
+      <c r="A20" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="28">
-        <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" ht="15.75" spans="1:5">
-      <c r="A16" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-    </row>
-    <row r="17" ht="15.75" spans="1:5">
-      <c r="A17" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" ht="15.75" spans="1:5">
-      <c r="A18" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" ht="15.75" spans="1:5">
-      <c r="A19" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" ht="15.75" spans="1:5">
-      <c r="A20" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="30" t="s">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" ht="15.75" spans="1:5">
+      <c r="A21" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="29">
+        <f>SUM(E3:E15)</f>
         <v>8</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-    </row>
-    <row r="21" ht="15.75" spans="1:5">
-      <c r="A21" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="31">
-        <f>SUM(E3:E15)</f>
-        <v>3</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="22"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" ht="15.75" spans="1:5">
-      <c r="A22" s="29"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="22"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="22"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="22"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" ht="15.75" spans="1:5">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" ht="15.75" spans="1:5">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
     </row>
     <row r="26" ht="15.75" spans="1:5">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
+      <c r="B26" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
     </row>
     <row r="27" ht="15.75" spans="1:5">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
+      <c r="B27" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
     </row>
     <row r="28" ht="15.75" spans="1:5">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
+      <c r="B28" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
     </row>
     <row r="30" ht="15.75" spans="1:5">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31" ht="15.75" spans="1:5">
-      <c r="A31" s="29"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
     </row>
     <row r="32" ht="15.75" spans="1:5">
-      <c r="A32" s="29"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
@@ -2320,7 +2316,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -2329,59 +2325,59 @@
     <col min="3" max="3" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="47.25" spans="1:4">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="1" customFormat="1" ht="31.5" spans="1:4">
+      <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="44" customHeight="1" spans="1:4">
-      <c r="A2" s="6" t="s">
+    <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
+      <c r="A2" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" s="2" customFormat="1" ht="44" customHeight="1" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
+      <c r="A3" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="44" customHeight="1" spans="1:4">
-      <c r="A4" s="6" t="s">
+      <c r="D3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
+      <c r="A4" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2403,47 +2399,47 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="12.4190476190476"/>
-    <col min="2" max="2" width="6.07619047619048" style="15"/>
+    <col min="2" max="2" width="6.07619047619048" style="13"/>
     <col min="3" max="3" width="41.7142857142857"/>
-    <col min="4" max="4" width="6.07619047619048" style="19"/>
+    <col min="4" max="4" width="6.07619047619048" style="17"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D3" t="s">
@@ -2451,13 +2447,13 @@
       </c>
     </row>
     <row r="4" ht="45" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>53</v>
       </c>
       <c r="D4" t="s">
@@ -2465,13 +2461,13 @@
       </c>
     </row>
     <row r="5" ht="30" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D5" t="s">
@@ -2479,13 +2475,13 @@
       </c>
     </row>
     <row r="6" ht="30" spans="1:4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D6" t="s">
@@ -2493,13 +2489,13 @@
       </c>
     </row>
     <row r="7" ht="30" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>60</v>
       </c>
       <c r="D7" t="s">
@@ -2507,13 +2503,13 @@
       </c>
     </row>
     <row r="8" ht="45" spans="1:4">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D8" t="s">
@@ -2521,13 +2517,13 @@
       </c>
     </row>
     <row r="9" ht="45" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>64</v>
       </c>
       <c r="D9" t="s">
@@ -2535,24 +2531,24 @@
       </c>
     </row>
     <row r="10" ht="45" spans="1:8">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="21"/>
+      <c r="D10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="22"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
@@ -2573,230 +2569,230 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9.99047619047619"/>
-    <col min="2" max="2" width="6.07619047619048" style="15"/>
+    <col min="2" max="2" width="6.07619047619048" style="13"/>
     <col min="3" max="3" width="43.2"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="4" ht="60" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5" ht="60" spans="1:3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" ht="30" spans="1:3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7" ht="45" spans="1:3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" ht="45" spans="1:3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="9" ht="45" spans="1:3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="10" ht="60" spans="1:3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" ht="30" spans="1:3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" ht="45" spans="1:3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="13" ht="45" spans="1:3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="14" ht="60" spans="1:3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" ht="60" spans="1:3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" ht="60" spans="1:3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="17" ht="60" spans="1:3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="18" ht="60" spans="1:3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="17" t="s">
+      <c r="B18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="19" ht="60" spans="1:3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="20" ht="45" spans="1:3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2819,372 +2815,372 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="10.6666666666667"/>
-    <col min="2" max="2" width="6.07619047619048" style="15"/>
+    <col min="2" max="2" width="6.07619047619048" style="13"/>
     <col min="3" max="3" width="51.9714285714286"/>
     <col min="4" max="4" width="9.99047619047619"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" ht="30" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" ht="30" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" ht="45" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" ht="45" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" ht="45" spans="1:4">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" ht="30" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" ht="45" spans="1:4">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" ht="45" spans="1:4">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="17" t="s">
+      <c r="B11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" ht="60" spans="1:4">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" ht="30" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" ht="30" spans="1:4">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" ht="30" spans="1:4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" ht="30" spans="1:4">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" ht="30" spans="1:4">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="17" t="s">
+      <c r="B17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" ht="30" spans="1:4">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" ht="45" spans="1:4">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="20" ht="30" spans="1:4">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" ht="30" spans="1:4">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="B21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" ht="30" spans="1:4">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="18" t="s">
+      <c r="B22" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" ht="30" spans="1:4">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="B23" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" ht="30" spans="1:4">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B24" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" ht="30" spans="1:4">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="26" ht="45" spans="1:4">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3214,97 +3210,97 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" ht="45" spans="1:4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" ht="30" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" ht="30" spans="1:4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" ht="30" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>166</v>
       </c>
       <c r="D7" t="s">
@@ -3312,13 +3308,13 @@
       </c>
     </row>
     <row r="8" ht="30" spans="1:4">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>168</v>
       </c>
       <c r="D8" t="s">
@@ -3326,13 +3322,13 @@
       </c>
     </row>
     <row r="9" ht="30" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>170</v>
       </c>
       <c r="D9" t="s">
@@ -3367,16 +3363,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3385,7 +3381,7 @@
         <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>172</v>
@@ -3409,8 +3405,8 @@
   <sheetPr/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3421,290 +3417,266 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="45" spans="1:4">
-      <c r="A2" s="7" t="s">
+    <row r="2" s="1" customFormat="1" ht="45" spans="1:4">
+      <c r="A2" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" ht="45" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" ht="60" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" ht="45" spans="1:4">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" ht="45" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" ht="30" spans="1:4">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" ht="45" spans="1:4">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" ht="60" spans="1:4">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" ht="45" spans="1:4">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" ht="45" spans="1:4">
+      <c r="A12" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" ht="45" spans="1:4">
-      <c r="A12" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" ht="45" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" ht="45" spans="1:4">
-      <c r="A13" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" ht="30" spans="1:4">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" ht="45" spans="1:4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" ht="60" spans="1:4">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="12" t="s">
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" ht="45" spans="1:4">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" ht="45" spans="1:4">
-      <c r="A18" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" ht="45" spans="1:4">
-      <c r="A19" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" ht="45" spans="1:4">
-      <c r="A20" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="D17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="7"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
@@ -3729,66 +3701,66 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="95" customHeight="1" spans="1:4">
-      <c r="A2" s="6" t="s">
+    <row r="2" s="1" customFormat="1" ht="95" customHeight="1" spans="1:4">
+      <c r="A2" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" s="2" customFormat="1" ht="45" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="45" spans="1:4">
+      <c r="A3" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="93" customHeight="1" spans="1:4">
-      <c r="A4" s="6" t="s">
+      <c r="D3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="93" customHeight="1" spans="1:4">
+      <c r="A4" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="7"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -3814,58 +3786,58 @@
   </cols>
   <sheetData>
     <row r="1" ht="31.5" spans="1:4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="44" customHeight="1" spans="1:4">
-      <c r="A2" s="6" t="s">
+    <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
+      <c r="A2" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" s="2" customFormat="1" ht="33" customHeight="1" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="33" customHeight="1" spans="1:4">
+      <c r="A3" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" s="2" customFormat="1" ht="34" customHeight="1" spans="1:4">
-      <c r="A4" s="6" t="s">
+      <c r="D3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="34" customHeight="1" spans="1:4">
+      <c r="A4" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PDP Test scripts updated
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="987" activeTab="9"/>
+    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="987" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -666,6 +666,78 @@
     <t>Free shipping to all countries but not shippable to US: Ensure that the items which are shippable to other countries are not shippable to US.</t>
   </si>
   <si>
+    <t>IGP_TC_241</t>
+  </si>
+  <si>
+    <t>Fields are present: Ensure that all the respective fields should be visible.</t>
+  </si>
+  <si>
+    <t>IGP_TC_242</t>
+  </si>
+  <si>
+    <t>Check Image fields: Ensure that image fields are present.</t>
+  </si>
+  <si>
+    <t>IGP_TC_243</t>
+  </si>
+  <si>
+    <t>Error message for International Deliveries: Ensure that international delivery not possible for Flowers.</t>
+  </si>
+  <si>
+    <t>IGP_TC_244</t>
+  </si>
+  <si>
+    <t>Error message for International Deliveries: Ensure that international delivery not possible for Cakes.</t>
+  </si>
+  <si>
+    <t>IGP_TC_245</t>
+  </si>
+  <si>
+    <t>Delivery Options visibility: All the 3 delivery options should be visbile.</t>
+  </si>
+  <si>
+    <t>IGP_TC_246</t>
+  </si>
+  <si>
+    <t>Fixed Date delivery:Ensure that the user selects the Fix Date delivery option.</t>
+  </si>
+  <si>
+    <t>IGP_TC_247</t>
+  </si>
+  <si>
+    <t>Fixed time delivery:Ensure that the user selects the Fixed time delivery option.</t>
+  </si>
+  <si>
+    <t>IGP_TC_248</t>
+  </si>
+  <si>
+    <t>Midnight Delivery:Ensure that the user selects the Midnight Delivery option.</t>
+  </si>
+  <si>
+    <t>IGP_TC_249</t>
+  </si>
+  <si>
+    <t>Product Description tab: Verify that Product Description tab is visible.</t>
+  </si>
+  <si>
+    <t>IGP_TC_250</t>
+  </si>
+  <si>
+    <t>Similar Gift Recommendations: Verify that Similar Gift Recommendations heading is visible.</t>
+  </si>
+  <si>
+    <t>IGP_TC_251</t>
+  </si>
+  <si>
+    <t>Footer: Verify that Similar Gift Recommendations heading is visible.</t>
+  </si>
+  <si>
+    <t>IGP_TC_252</t>
+  </si>
+  <si>
+    <t>Buy Now: Check the functionality of Buy Now button.</t>
+  </si>
+  <si>
     <t>IGP_TC_232</t>
   </si>
   <si>
@@ -725,10 +797,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -803,72 +875,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -884,10 +890,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -899,9 +942,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -909,6 +967,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -922,23 +987,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -972,13 +1044,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,7 +1062,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1002,19 +1092,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,7 +1110,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1044,7 +1164,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1062,97 +1212,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,17 +1268,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1230,7 +1307,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1250,41 +1342,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1293,143 +1350,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1915,7 +1987,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2061,7 +2133,7 @@
       </c>
       <c r="E8" s="26">
         <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2202,7 +2274,7 @@
       </c>
       <c r="B21" s="29">
         <f>SUM(E3:E15)</f>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2315,7 +2387,7 @@
   <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2341,13 +2413,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -2355,13 +2427,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -2369,13 +2441,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -3403,15 +3475,16 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="8.1047619047619"/>
+    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="8.1047619047619"/>
     <col min="3" max="3" width="43.3333333333333"/>
     <col min="4" max="1025" width="8.1047619047619"/>
   </cols>
@@ -3654,29 +3727,197 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="5"/>
+    <row r="18" ht="30" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" ht="30" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" ht="45" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" ht="45" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" ht="30" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" ht="30" spans="1:4">
+      <c r="A23" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" ht="30" spans="1:4">
+      <c r="A24" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" ht="30" spans="1:4">
+      <c r="A25" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" ht="30" spans="1:4">
+      <c r="A26" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" ht="45" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" ht="30" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" ht="30" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
@@ -3716,13 +3957,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="95" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -3730,13 +3971,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="45" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -3744,13 +3985,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="93" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -3801,13 +4042,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -3815,13 +4056,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="33" customHeight="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -3829,13 +4070,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="34" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
PDP Test Cases and Test Scripts updated
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="987" activeTab="6"/>
+    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="AppControl" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253">
   <si>
     <t>Project ID/Name</t>
   </si>
@@ -738,6 +738,24 @@
     <t>Buy Now: Check the functionality of Buy Now button.</t>
   </si>
   <si>
+    <t>IGP_TC_253</t>
+  </si>
+  <si>
+    <t>Add to Cart: Ensure that the product is added to cart upon clicking 'Add to cart' button.</t>
+  </si>
+  <si>
+    <t>IGP_TC_254</t>
+  </si>
+  <si>
+    <t>Product variety: Ensure that user select product with different varities.</t>
+  </si>
+  <si>
+    <t>IGP_TC_255</t>
+  </si>
+  <si>
+    <t>Choose Type of Base: Ensure that user select the base.</t>
+  </si>
+  <si>
     <t>IGP_TC_232</t>
   </si>
   <si>
@@ -797,10 +815,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -868,14 +886,58 @@
       <charset val="1"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -890,14 +952,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -913,7 +977,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -921,22 +992,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -950,54 +1005,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1010,7 +1021,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1044,7 +1062,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1057,6 +1093,60 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1080,55 +1170,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,37 +1182,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1188,31 +1206,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1225,6 +1225,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1270,10 +1288,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1283,7 +1299,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1303,11 +1319,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1327,21 +1375,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1350,158 +1383,143 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1986,8 +2004,8 @@
   <sheetPr/>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2133,7 +2151,7 @@
       </c>
       <c r="E8" s="26">
         <f>IF(B8="Y",COUNTIF(Suite6!B2:B52,"Y"),0)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2141,7 +2159,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>9</v>
@@ -2158,7 +2176,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>9</v>
@@ -2175,7 +2193,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>9</v>
@@ -2274,7 +2292,7 @@
       </c>
       <c r="B21" s="29">
         <f>SUM(E3:E15)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
@@ -2413,13 +2431,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -2427,13 +2445,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -2441,13 +2459,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -3477,8 +3495,8 @@
   <sheetPr/>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -3634,7 +3652,7 @@
         <v>191</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>192</v>
@@ -3676,7 +3694,7 @@
         <v>197</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>198</v>
@@ -3690,7 +3708,7 @@
         <v>199</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>200</v>
@@ -3704,7 +3722,7 @@
         <v>201</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>202</v>
@@ -3718,7 +3736,7 @@
         <v>203</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>204</v>
@@ -3895,23 +3913,47 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="5"/>
+    <row r="30" ht="30" spans="1:4">
+      <c r="A30" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" ht="30" spans="1:4">
+      <c r="A31" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" ht="30" spans="1:4">
+      <c r="A32" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="5"/>
@@ -3957,13 +3999,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="95" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -3971,13 +4013,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="45" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -3985,13 +4027,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="93" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>
@@ -4042,13 +4084,13 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="44" customHeight="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>49</v>
@@ -4056,13 +4098,13 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="33" customHeight="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -4070,13 +4112,13 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="34" customHeight="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>49</v>

</xml_diff>